<commit_message>
Review GPIO & TAIL_module CCDs and update GDD review sheet Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specifications/Architecture/GDD/Review.xlsx
+++ b/Software Specifications/Architecture/GDD/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>Review point</t>
   </si>
@@ -80,13 +80,27 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>FYI: it shall be TiRight_u8GetStatus but it's a 
+minor point</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>for u8Pin range shall be --&gt; 0 - 43 (put here the max num of pins)
+Also LED_1, LED_2 point still open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +166,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,7 +1123,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1141,7 +1157,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1317,14 +1332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1334,7 +1349,7 @@
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1354,7 +1369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="5">
         <v>43924</v>
       </c>
@@ -1364,12 +1379,14 @@
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75">
       <c r="A3" s="5">
         <v>43924</v>
       </c>
@@ -1379,12 +1396,14 @@
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="5">
         <v>43924</v>
       </c>
@@ -1394,12 +1413,14 @@
       <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="90">
       <c r="A5" s="5">
         <v>43924</v>
       </c>
@@ -1409,12 +1430,17 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5">
         <v>43924</v>
       </c>
@@ -1424,12 +1450,14 @@
       <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75">
       <c r="A7" s="5">
         <v>43924</v>
       </c>
@@ -1441,10 +1469,13 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="5">
         <v>43924</v>
       </c>
@@ -1454,12 +1485,14 @@
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="90">
       <c r="A9" s="5">
         <v>43924</v>
       </c>
@@ -1469,12 +1502,14 @@
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="5">
         <v>43924</v>
       </c>
@@ -1484,12 +1519,14 @@
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60">
       <c r="A11" s="5">
         <v>43924</v>
       </c>
@@ -1499,7 +1536,9 @@
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>